<commit_message>
push code CRUD kho
</commit_message>
<xml_diff>
--- a/src/Excel/Products.xlsx
+++ b/src/Excel/Products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maccuacu/Desktop/da1/QuanlyChuoiCH/src/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DuAn1_Java_PTPM\Du_an_1\DuAn1Nhom3\src\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF333806-4C68-1748-B0D6-BFF3765FEC78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B149F4F3-3A69-4F3E-8500-192E554E5090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="1400" windowWidth="28040" windowHeight="17440" xr2:uid="{862D2307-B0B9-A248-9588-08AF73614AFD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{862D2307-B0B9-A248-9588-08AF73614AFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -412,19 +412,19 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
fix login, fix import file excel
</commit_message>
<xml_diff>
--- a/src/Excel/Products.xlsx
+++ b/src/Excel/Products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DuAn1_Java_PTPM\Du_an_1\DuAn1Nhom3\src\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maccuacu/Desktop/da1/QuanlyChuoiCH/src/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2E8B04-3705-4006-BEFA-BFD74EB8512E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADDAF0F-22BA-5A4C-9835-13B58CE42F5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{862D2307-B0B9-A248-9588-08AF73614AFD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19640" xr2:uid="{862D2307-B0B9-A248-9588-08AF73614AFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Code</t>
   </si>
@@ -69,9 +66,6 @@
     <t>Nguồn gốc 1</t>
   </si>
   <si>
-    <t>7E90870D-89E3-4AEB-9130-176566081D76</t>
-  </si>
-  <si>
     <t>SP010</t>
   </si>
   <si>
@@ -96,45 +90,24 @@
     <t>Nguồn gốc 2</t>
   </si>
   <si>
-    <t>7E90870D-89E3-4AEB-9130-176566081D77</t>
-  </si>
-  <si>
     <t>Nguồn gốc 3</t>
   </si>
   <si>
-    <t>7E90870D-89E3-4AEB-9130-176566081D78</t>
-  </si>
-  <si>
     <t>Nguồn gốc 4</t>
   </si>
   <si>
-    <t>7E90870D-89E3-4AEB-9130-176566081D79</t>
-  </si>
-  <si>
     <t>Nguồn gốc 5</t>
   </si>
   <si>
-    <t>7E90870D-89E3-4AEB-9130-176566081D80</t>
-  </si>
-  <si>
     <t>Nguồn gốc 6</t>
   </si>
   <si>
-    <t>7E90870D-89E3-4AEB-9130-176566081D81</t>
-  </si>
-  <si>
     <t>Nguồn gốc 7</t>
   </si>
   <si>
-    <t>7E90870D-89E3-4AEB-9130-176566081D82</t>
-  </si>
-  <si>
     <t>Nguồn gốc 8</t>
   </si>
   <si>
-    <t>7E90870D-89E3-4AEB-9130-176566081D83</t>
-  </si>
-  <si>
     <t>SP2</t>
   </si>
   <si>
@@ -151,12 +124,39 @@
   </si>
   <si>
     <t>SP7</t>
+  </si>
+  <si>
+    <t>ff9f0d7b-41ef-482a-9e84-2b81e7aa6e29</t>
+  </si>
+  <si>
+    <t>ff9f0d7b-41ef-482a-9e84-2b81e7aa6e30</t>
+  </si>
+  <si>
+    <t>ff9f0d7b-41ef-482a-9e84-2b81e7aa6e31</t>
+  </si>
+  <si>
+    <t>ff9f0d7b-41ef-482a-9e84-2b81e7aa6e32</t>
+  </si>
+  <si>
+    <t>ff9f0d7b-41ef-482a-9e84-2b81e7aa6e33</t>
+  </si>
+  <si>
+    <t>ff9f0d7b-41ef-482a-9e84-2b81e7aa6e34</t>
+  </si>
+  <si>
+    <t>ff9f0d7b-41ef-482a-9e84-2b81e7aa6e35</t>
+  </si>
+  <si>
+    <t>ff9f0d7b-41ef-482a-9e84-2b81e7aa6e36</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -192,10 +192,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,22 +511,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65306FBD-D576-1D47-9A7B-B8C8FCBA4E34}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,263 +557,260 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2">
+        <v>100000</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44511</v>
+      </c>
+      <c r="F2" s="1">
+        <v>44512</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1">
+        <v>44512</v>
+      </c>
+      <c r="I2" s="1">
+        <v>44512</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="E2">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2">
         <v>100000</v>
       </c>
-      <c r="F2" s="1">
-        <v>44511</v>
-      </c>
-      <c r="G2" s="1">
-        <v>44511</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="E3" s="1">
+        <v>44512</v>
+      </c>
+      <c r="F3" s="1">
+        <v>44513</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="1">
+        <v>44513</v>
+      </c>
+      <c r="I3" s="1">
+        <v>44513</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1">
-        <v>44511</v>
-      </c>
-      <c r="J2" s="1">
-        <v>44511</v>
-      </c>
-      <c r="K2" s="1">
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2">
+        <v>100000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44513</v>
+      </c>
+      <c r="F4" s="1">
+        <v>44514</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="1">
+        <v>44514</v>
+      </c>
+      <c r="I4" s="1">
+        <v>44514</v>
+      </c>
+      <c r="J4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="E3">
-        <v>100001</v>
-      </c>
-      <c r="F3" s="1">
-        <v>44511</v>
-      </c>
-      <c r="G3" s="1">
-        <v>44511</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="D5" s="2">
+        <v>100000</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44514</v>
+      </c>
+      <c r="F5" s="1">
+        <v>44515</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="1">
+        <v>44515</v>
+      </c>
+      <c r="I5" s="1">
+        <v>44515</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="1">
-        <v>44511</v>
-      </c>
-      <c r="J3" s="1">
-        <v>44511</v>
-      </c>
-      <c r="K3" s="1">
+      <c r="D6" s="2">
+        <v>100000</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44515</v>
+      </c>
+      <c r="F6" s="1">
+        <v>44516</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="1">
+        <v>44516</v>
+      </c>
+      <c r="I6" s="1">
+        <v>44516</v>
+      </c>
+      <c r="J6" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="E4">
-        <v>100002</v>
-      </c>
-      <c r="F4" s="1">
-        <v>44511</v>
-      </c>
-      <c r="G4" s="1">
-        <v>44511</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="D7" s="2">
+        <v>100000</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44516</v>
+      </c>
+      <c r="F7" s="1">
+        <v>44517</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="1">
+        <v>44517</v>
+      </c>
+      <c r="I7" s="1">
+        <v>44517</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="1">
-        <v>44511</v>
-      </c>
-      <c r="J4" s="1">
-        <v>44511</v>
-      </c>
-      <c r="K4" s="1">
+      <c r="D8" s="2">
+        <v>100000</v>
+      </c>
+      <c r="E8" s="1">
+        <v>44517</v>
+      </c>
+      <c r="F8" s="1">
+        <v>44518</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="1">
+        <v>44518</v>
+      </c>
+      <c r="I8" s="1">
+        <v>44518</v>
+      </c>
+      <c r="J8" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="E5">
-        <v>100003</v>
-      </c>
-      <c r="F5" s="1">
-        <v>44511</v>
-      </c>
-      <c r="G5" s="1">
-        <v>44511</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="1">
-        <v>44511</v>
-      </c>
-      <c r="J5" s="1">
-        <v>44511</v>
-      </c>
-      <c r="K5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6">
-        <v>100004</v>
-      </c>
-      <c r="F6" s="1">
-        <v>44511</v>
-      </c>
-      <c r="G6" s="1">
-        <v>44511</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="1">
-        <v>44511</v>
-      </c>
-      <c r="J6" s="1">
-        <v>44511</v>
-      </c>
-      <c r="K6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7">
-        <v>100005</v>
-      </c>
-      <c r="F7" s="1">
-        <v>44511</v>
-      </c>
-      <c r="G7" s="1">
-        <v>44511</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="1">
-        <v>44511</v>
-      </c>
-      <c r="J7" s="1">
-        <v>44511</v>
-      </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D9" s="2">
+        <v>100000</v>
+      </c>
+      <c r="E9" s="1">
+        <v>44518</v>
+      </c>
+      <c r="F9" s="1">
+        <v>44519</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8">
-        <v>100006</v>
-      </c>
-      <c r="F8" s="1">
-        <v>44511</v>
-      </c>
-      <c r="G8" s="1">
-        <v>44511</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="1">
-        <v>44511</v>
-      </c>
-      <c r="J8" s="1">
-        <v>44511</v>
-      </c>
-      <c r="K8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9">
-        <v>100007</v>
-      </c>
-      <c r="F9" s="1">
-        <v>44511</v>
-      </c>
-      <c r="G9" s="1">
-        <v>44511</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>35</v>
+      <c r="H9" s="1">
+        <v>44519</v>
       </c>
       <c r="I9" s="1">
-        <v>44511</v>
-      </c>
-      <c r="J9" s="1">
-        <v>44511</v>
-      </c>
-      <c r="K9" s="1">
+        <v>44519</v>
+      </c>
+      <c r="J9" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update CRUD cuaHang; repository
</commit_message>
<xml_diff>
--- a/src/Excel/Products.xlsx
+++ b/src/Excel/Products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DuAn1_Java_PTPM\Du_an_1\DuAn1Nhom3\src\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95181F9B-4CFD-4265-BE14-0E3F4A968B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23DC623-022C-46F0-B387-0568C561AC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{862D2307-B0B9-A248-9588-08AF73614AFD}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Code</t>
   </si>
@@ -158,7 +155,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -195,10 +192,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,22 +511,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65306FBD-D576-1D47-9A7B-B8C8FCBA4E34}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J9"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -559,241 +557,261 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>100000</v>
+      </c>
+      <c r="E2" s="2">
+        <v>44511</v>
+      </c>
+      <c r="F2" s="2">
+        <v>44511</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2">
-        <v>100000</v>
-      </c>
-      <c r="F2" s="2">
-        <v>44511</v>
-      </c>
-      <c r="G2" s="2">
-        <v>44511</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2">
+        <v>44511</v>
+      </c>
+      <c r="I2" s="2">
+        <v>44511</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2">
-        <v>44511</v>
-      </c>
-      <c r="J2" s="2">
-        <v>44511</v>
-      </c>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3">
+        <v>21</v>
+      </c>
+      <c r="D3">
         <v>100001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>44512</v>
       </c>
       <c r="F3" s="2">
         <v>44512</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="2">
+        <v>44511</v>
+      </c>
+      <c r="I3" s="2">
         <v>44512</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="2">
-        <v>44511</v>
-      </c>
-      <c r="J3" s="2">
-        <v>44512</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4">
+      <c r="D4">
         <v>100002</v>
+      </c>
+      <c r="E4" s="2">
+        <v>44513</v>
       </c>
       <c r="F4" s="2">
         <v>44513</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="2">
+        <v>44511</v>
+      </c>
+      <c r="I4" s="2">
         <v>44513</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="2">
-        <v>44511</v>
-      </c>
-      <c r="J4" s="2">
-        <v>44513</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5">
+      <c r="D5">
         <v>100003</v>
+      </c>
+      <c r="E5" s="2">
+        <v>44514</v>
       </c>
       <c r="F5" s="2">
         <v>44514</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="2">
+        <v>44511</v>
+      </c>
+      <c r="I5" s="2">
         <v>44514</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="2">
-        <v>44511</v>
-      </c>
-      <c r="J5" s="2">
-        <v>44514</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6">
+      <c r="D6">
         <v>100004</v>
+      </c>
+      <c r="E6" s="2">
+        <v>44515</v>
       </c>
       <c r="F6" s="2">
         <v>44515</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="2">
+        <v>44511</v>
+      </c>
+      <c r="I6" s="2">
         <v>44515</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="2">
-        <v>44511</v>
-      </c>
-      <c r="J6" s="2">
-        <v>44515</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7">
+      <c r="D7">
         <v>100005</v>
+      </c>
+      <c r="E7" s="2">
+        <v>44516</v>
       </c>
       <c r="F7" s="2">
         <v>44516</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="2">
+        <v>44511</v>
+      </c>
+      <c r="I7" s="2">
         <v>44516</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="2">
-        <v>44511</v>
-      </c>
-      <c r="J7" s="2">
-        <v>44516</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8">
+      <c r="D8">
         <v>100006</v>
+      </c>
+      <c r="E8" s="2">
+        <v>44517</v>
       </c>
       <c r="F8" s="2">
         <v>44517</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="2">
+        <v>44511</v>
+      </c>
+      <c r="I8" s="2">
         <v>44517</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="J8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="2">
-        <v>44511</v>
-      </c>
-      <c r="J8" s="2">
-        <v>44517</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9">
+      <c r="D9">
         <v>100007</v>
+      </c>
+      <c r="E9" s="2">
+        <v>44518</v>
       </c>
       <c r="F9" s="2">
         <v>44518</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="2">
+        <v>44511</v>
+      </c>
+      <c r="I9" s="2">
         <v>44518</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="2">
-        <v>44511</v>
-      </c>
-      <c r="J9" s="2">
-        <v>44518</v>
+      <c r="J9" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>